<commit_message>
Fixed bug where rating=0 was impossible due to the order of IFS conditions
</commit_message>
<xml_diff>
--- a/excel_backward_compatible/DPR Tactics Calculator.xlsx
+++ b/excel_backward_compatible/DPR Tactics Calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\GitHub-personal\claire-puppylove\dnd-5e-dpr-tactics-calculator\excel_backward_compatible\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8CCD920-25AE-48EC-9E44-2587086C5795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BB70F0-31D4-4418-B288-E0B583A50C84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1823,6 +1823,19 @@
       <font>
         <b/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="168" formatCode="0_ "/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1853,37 +1866,31 @@
       <numFmt numFmtId="167" formatCode="0.00_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="174" formatCode="0.000_ "/>
+      <numFmt numFmtId="169" formatCode="0.000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode="0.0000_ "/>
+      <numFmt numFmtId="170" formatCode="0.0000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode="0.00000_ "/>
+      <numFmt numFmtId="171" formatCode="0.00000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="171" formatCode="0.000000_ "/>
+      <numFmt numFmtId="172" formatCode="0.000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode="0.0000000_ "/>
+      <numFmt numFmtId="173" formatCode="0.0000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
@@ -1896,7 +1903,12 @@
       <font>
         <b/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -1907,7 +1919,7 @@
       <font>
         <b/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -1918,7 +1930,7 @@
       <font>
         <b/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -1929,18 +1941,7 @@
       <font>
         <b/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -1952,19 +1953,19 @@
       <numFmt numFmtId="168" formatCode="0_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -1985,38 +1986,38 @@
       <alignment horizontal="center" wrapText="1"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="0_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -2027,25 +2028,25 @@
       <numFmt numFmtId="165" formatCode="\+0;\-0;0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -2063,28 +2064,28 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <numFmt numFmtId="168" formatCode="0_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -2129,22 +2130,22 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
     </dxf>
     <dxf>
       <font>
@@ -2152,7 +2153,7 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="0.00000000_ "/>
+      <numFmt numFmtId="174" formatCode="0.00000000_ "/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
@@ -4489,6 +4490,12 @@
     <dataField name="DPR Total Rating" fld="69" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="8">
+    <format dxfId="15">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="14">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
     <format dxfId="13">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
@@ -4505,12 +4512,6 @@
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
     <format dxfId="8">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="7">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="6">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -4690,10 +4691,32 @@
     <tableColumn id="66" xr3:uid="{00000000-0010-0000-0000-000042000000}" name="Total Damage per Round" dataDxfId="19">
       <calculatedColumnFormula>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="DPR per Target Rating" dataDxfId="18">
-      <calculatedColumnFormula>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</calculatedColumnFormula>
+    <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="DPR per Target Rating" dataDxfId="1">
+      <calculatedColumnFormula array="1">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="DPR Rating per Target Description" dataDxfId="17">
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="DPR Rating per Target Description" dataDxfId="18">
       <calculatedColumnFormula array="1">_xlfn.IFS(
     ISNUMBER(DPRTacticsCalculator[[#This Row],[DPR per Target Rating]])=FALSE,"-",
     DPRTacticsCalculator[[#This Row],[DPR per Target Rating]]=0,"☆☆☆☆  No damage",
@@ -4704,10 +4727,32 @@
     DPRTacticsCalculator[[#This Row],[DPR per Target Rating]]=5,"🕱🕱🕱🕱🕱  Deadly"
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="Total DPR Rating" dataDxfId="16">
-      <calculatedColumnFormula>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</calculatedColumnFormula>
+    <tableColumn id="71" xr3:uid="{00000000-0010-0000-0000-000047000000}" name="Total DPR Rating" dataDxfId="0">
+      <calculatedColumnFormula array="1">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="Total DPR Rating Description" dataDxfId="15">
+    <tableColumn id="70" xr3:uid="{00000000-0010-0000-0000-000046000000}" name="Total DPR Rating Description" dataDxfId="17">
       <calculatedColumnFormula array="1">_xlfn.IFS(
     ISNUMBER(DPRTacticsCalculator[[#This Row],[Total DPR Rating]])=FALSE,"-",
     DPRTacticsCalculator[[#This Row],[Total DPR Rating]]=0,"☆☆☆☆  No damage",
@@ -4718,7 +4763,7 @@
     DPRTacticsCalculator[[#This Row],[Total DPR Rating]]=5,"🕱🕱🕱🕱🕱  Deadly"
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Notes" dataDxfId="14"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="Notes" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -4728,18 +4773,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="DPRRatingExplanation" displayName="DPRRatingExplanation" ref="A1:F21" totalsRowShown="0">
   <autoFilter ref="A1:F21" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CR or LV" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Max Expected _x000a_Enemy HP" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Low DPR _x000a_Threshold" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="CR or LV" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Max Expected _x000a_Enemy HP" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Low DPR _x000a_Threshold" dataDxfId="5">
       <calculatedColumnFormula>$B2/I$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Target DPR _x000a_Threshold" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Target DPR _x000a_Threshold" dataDxfId="4">
       <calculatedColumnFormula>$B2/J$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="High DPR _x000a_Threshold" dataDxfId="1">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="High DPR _x000a_Threshold" dataDxfId="3">
       <calculatedColumnFormula>$B2/K$2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="OP DPR _x000a_Threshold" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="OP DPR _x000a_Threshold" dataDxfId="2">
       <calculatedColumnFormula>$B2/L$2</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5568,8 +5613,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP2" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP2" s="35" t="str" cm="1">
+        <f t="array" ref="BP2">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ2" s="24" t="str" cm="1">
@@ -5584,8 +5651,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR2" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR2" s="33" t="str" cm="1">
+        <f t="array" ref="BR2">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS2" s="24" t="str" cm="1">
@@ -5873,8 +5962,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>10.26</v>
       </c>
-      <c r="BP3" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP3" s="35" cm="1">
+        <f t="array" ref="BP3">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>2</v>
       </c>
       <c r="BQ3" s="24" t="str" cm="1">
@@ -5889,8 +6000,30 @@
 )</f>
         <v>★★☆☆  Low (support, control, debuff)</v>
       </c>
-      <c r="BR3" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR3" s="33" cm="1">
+        <f t="array" ref="BR3">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>2</v>
       </c>
       <c r="BS3" s="24" t="str" cm="1">
@@ -6178,8 +6311,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP4" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP4" s="35" t="str" cm="1">
+        <f t="array" ref="BP4">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ4" s="24" t="str" cm="1">
@@ -6194,8 +6349,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR4" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR4" s="33" t="str" cm="1">
+        <f t="array" ref="BR4">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS4" s="24" t="str" cm="1">
@@ -6483,8 +6660,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>13.647500000000001</v>
       </c>
-      <c r="BP5" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP5" s="35" cm="1">
+        <f t="array" ref="BP5">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>3</v>
       </c>
       <c r="BQ5" s="24" t="str" cm="1">
@@ -6499,8 +6698,30 @@
 )</f>
         <v>★★★☆  Target (expected)</v>
       </c>
-      <c r="BR5" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR5" s="33" cm="1">
+        <f t="array" ref="BR5">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>3</v>
       </c>
       <c r="BS5" s="24" t="str" cm="1">
@@ -6788,8 +7009,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP6" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP6" s="35" t="str" cm="1">
+        <f t="array" ref="BP6">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ6" s="24" t="str" cm="1">
@@ -6804,8 +7047,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR6" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR6" s="33" t="str" cm="1">
+        <f t="array" ref="BR6">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS6" s="24" t="str" cm="1">
@@ -7093,8 +7358,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>25.740000000000002</v>
       </c>
-      <c r="BP7" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP7" s="35" cm="1">
+        <f t="array" ref="BP7">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>4</v>
       </c>
       <c r="BQ7" s="24" t="str" cm="1">
@@ -7109,8 +7396,30 @@
 )</f>
         <v>★★★★  High (heavy hitter)</v>
       </c>
-      <c r="BR7" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR7" s="33" cm="1">
+        <f t="array" ref="BR7">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>4</v>
       </c>
       <c r="BS7" s="24" t="str" cm="1">
@@ -7398,8 +7707,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>119</v>
       </c>
-      <c r="BP8" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP8" s="35" cm="1">
+        <f t="array" ref="BP8">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>3</v>
       </c>
       <c r="BQ8" s="24" t="str" cm="1">
@@ -7414,8 +7745,30 @@
 )</f>
         <v>★★★☆  Target (expected)</v>
       </c>
-      <c r="BR8" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR8" s="33" cm="1">
+        <f t="array" ref="BR8">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>5</v>
       </c>
       <c r="BS8" s="24" t="str" cm="1">
@@ -7703,8 +8056,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>124.66666666666666</v>
       </c>
-      <c r="BP9" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP9" s="35" cm="1">
+        <f t="array" ref="BP9">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>3</v>
       </c>
       <c r="BQ9" s="24" t="str" cm="1">
@@ -7719,8 +8094,30 @@
 )</f>
         <v>★★★☆  Target (expected)</v>
       </c>
-      <c r="BR9" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR9" s="33" cm="1">
+        <f t="array" ref="BR9">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>5</v>
       </c>
       <c r="BS9" s="24" t="str" cm="1">
@@ -8008,8 +8405,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>133.69999999999999</v>
       </c>
-      <c r="BP10" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP10" s="35" cm="1">
+        <f t="array" ref="BP10">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>3</v>
       </c>
       <c r="BQ10" s="24" t="str" cm="1">
@@ -8024,8 +8443,30 @@
 )</f>
         <v>★★★☆  Target (expected)</v>
       </c>
-      <c r="BR10" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR10" s="33" cm="1">
+        <f t="array" ref="BR10">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>5</v>
       </c>
       <c r="BS10" s="24" t="str" cm="1">
@@ -8313,8 +8754,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>8.4500000000000011</v>
       </c>
-      <c r="BP11" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP11" s="35" cm="1">
+        <f t="array" ref="BP11">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>2</v>
       </c>
       <c r="BQ11" s="24" t="str" cm="1">
@@ -8329,8 +8792,30 @@
 )</f>
         <v>★★☆☆  Low (support, control, debuff)</v>
       </c>
-      <c r="BR11" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR11" s="33" cm="1">
+        <f t="array" ref="BR11">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>2</v>
       </c>
       <c r="BS11" s="24" t="str" cm="1">
@@ -8618,8 +9103,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP12" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP12" s="35" t="str" cm="1">
+        <f t="array" ref="BP12">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ12" s="24" t="str" cm="1">
@@ -8634,8 +9141,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR12" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR12" s="33" t="str" cm="1">
+        <f t="array" ref="BR12">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS12" s="24" t="str" cm="1">
@@ -8923,8 +9452,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP13" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP13" s="35" t="str" cm="1">
+        <f t="array" ref="BP13">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ13" s="24" t="str" cm="1">
@@ -8939,8 +9490,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR13" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR13" s="33" t="str" cm="1">
+        <f t="array" ref="BR13">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS13" s="24" t="str" cm="1">
@@ -9228,8 +9801,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP14" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP14" s="35" t="str" cm="1">
+        <f t="array" ref="BP14">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ14" s="24" t="str" cm="1">
@@ -9244,8 +9839,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR14" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR14" s="33" t="str" cm="1">
+        <f t="array" ref="BR14">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS14" s="24" t="str" cm="1">
@@ -9533,8 +10150,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>8.5556250000000009</v>
       </c>
-      <c r="BP15" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP15" s="35" cm="1">
+        <f t="array" ref="BP15">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>2</v>
       </c>
       <c r="BQ15" s="24" t="str" cm="1">
@@ -9549,8 +10188,30 @@
 )</f>
         <v>★★☆☆  Low (support, control, debuff)</v>
       </c>
-      <c r="BR15" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR15" s="33" cm="1">
+        <f t="array" ref="BR15">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>2</v>
       </c>
       <c r="BS15" s="24" t="str" cm="1">
@@ -9838,8 +10499,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP16" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP16" s="35" t="str" cm="1">
+        <f t="array" ref="BP16">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ16" s="24" t="str" cm="1">
@@ -9854,8 +10537,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR16" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR16" s="33" t="str" cm="1">
+        <f t="array" ref="BR16">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS16" s="24" t="str" cm="1">
@@ -10143,8 +10848,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP17" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP17" s="35" t="str" cm="1">
+        <f t="array" ref="BP17">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ17" s="24" t="str" cm="1">
@@ -10159,8 +10886,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR17" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR17" s="33" t="str" cm="1">
+        <f t="array" ref="BR17">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS17" s="24" t="str" cm="1">
@@ -10448,8 +11197,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP18" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP18" s="35" t="str" cm="1">
+        <f t="array" ref="BP18">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ18" s="24" t="str" cm="1">
@@ -10464,8 +11235,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR18" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR18" s="33" t="str" cm="1">
+        <f t="array" ref="BR18">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS18" s="24" t="str" cm="1">
@@ -10753,8 +11546,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP19" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP19" s="35" t="str" cm="1">
+        <f t="array" ref="BP19">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ19" s="24" t="str" cm="1">
@@ -10769,8 +11584,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR19" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR19" s="33" t="str" cm="1">
+        <f t="array" ref="BR19">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS19" s="24" t="str" cm="1">
@@ -11058,8 +11895,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP20" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP20" s="35" t="str" cm="1">
+        <f t="array" ref="BP20">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ20" s="24" t="str" cm="1">
@@ -11074,8 +11933,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR20" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR20" s="33" t="str" cm="1">
+        <f t="array" ref="BR20">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS20" s="24" t="str" cm="1">
@@ -11358,8 +12239,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>83.183333333333337</v>
       </c>
-      <c r="BP21" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP21" s="35" cm="1">
+        <f t="array" ref="BP21">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>3</v>
       </c>
       <c r="BQ21" s="24" t="str" cm="1">
@@ -11374,8 +12277,30 @@
 )</f>
         <v>★★★☆  Target (expected)</v>
       </c>
-      <c r="BR21" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR21" s="33" cm="1">
+        <f t="array" ref="BR21">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>5</v>
       </c>
       <c r="BS21" s="24" t="str" cm="1">
@@ -11658,8 +12583,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP22" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP22" s="35" t="str" cm="1">
+        <f t="array" ref="BP22">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ22" s="24" t="str" cm="1">
@@ -11674,8 +12621,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR22" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR22" s="33" t="str" cm="1">
+        <f t="array" ref="BR22">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS22" s="24" t="str" cm="1">
@@ -11958,8 +12927,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>24.404412500000003</v>
       </c>
-      <c r="BP23" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP23" s="35" cm="1">
+        <f t="array" ref="BP23">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>4</v>
       </c>
       <c r="BQ23" s="24" t="str" cm="1">
@@ -11974,8 +12965,30 @@
 )</f>
         <v>★★★★  High (heavy hitter)</v>
       </c>
-      <c r="BR23" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR23" s="33" cm="1">
+        <f t="array" ref="BR23">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>4</v>
       </c>
       <c r="BS23" s="24" t="str" cm="1">
@@ -12258,8 +13271,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>-</v>
       </c>
-      <c r="BP24" s="35" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP24" s="35" t="str" cm="1">
+        <f t="array" ref="BP24">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BQ24" s="24" t="str" cm="1">
@@ -12274,8 +13309,30 @@
 )</f>
         <v>-</v>
       </c>
-      <c r="BR24" s="33" t="str">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR24" s="33" t="str" cm="1">
+        <f t="array" ref="BR24">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>-</v>
       </c>
       <c r="BS24" s="24" t="str" cm="1">
@@ -12558,8 +13615,30 @@
         <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]]),(N("Only show if the tactic damage is showing a number")+N("Damage per round: Damage per tactic / number of rounds")+((N("Damage per tactic")+DPRTacticsCalculator[[#This Row],[Average Tactic Damage Total]])/(N("Number of rounds")+DPRTacticsCalculator[[#This Row],[Round]]))),"-")</f>
         <v>31.684485416666671</v>
       </c>
-      <c r="BP25" s="35">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),0),"-")</f>
+      <c r="BP25" s="35" cm="1">
+        <f t="array" ref="BP25">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Damage per Round per Target]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>4</v>
       </c>
       <c r="BQ25" s="24" t="str" cm="1">
@@ -12574,8 +13653,30 @@
 )</f>
         <v>★★★★  High (heavy hitter)</v>
       </c>
-      <c r="BR25" s="33">
-        <f>IF(ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),_xlfn.IFS((DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),5,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),4,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),3,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),2,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=(DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),1,(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),0),"-")</f>
+      <c r="BR25" s="33" cm="1">
+        <f t="array" ref="BR25">IF(
+    ISNUMBER(DPRTacticsCalculator[[#This Row],[Total Damage per Round]]),
+    _xlfn.IFS(
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]=0),
+            0,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/3)),
+            5,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/6)),
+            4,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/12)),
+            3,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&gt;
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            2,
+        (DPRTacticsCalculator[[#This Row],[Total Damage per Round]]&lt;=
+            (DPRTacticsCalculator[[#This Row],[Max Expected Enemy HP at CR or LV]]/24)),
+            1
+    ),
+    "-"
+)</f>
         <v>4</v>
       </c>
       <c r="BS25" s="24" t="str" cm="1">

</xml_diff>